<commit_message>
applicant and service app
</commit_message>
<xml_diff>
--- a/public/excelfile/serviceapplication.xlsx
+++ b/public/excelfile/serviceapplication.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abel.paul\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abel.paul\Desktop\NewNiwa\niwaebs\public\excelfile\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,51 +24,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>service_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> application_form_payment_status</t>
-  </si>
-  <si>
-    <t>date_of_inspection</t>
-  </si>
-  <si>
-    <t>service_type_id</t>
-  </si>
-  <si>
-    <t>current_step</t>
-  </si>
-  <si>
-    <t>mse_are_documents_verified</t>
-  </si>
-  <si>
-    <t>finance_is_application_fee_verified</t>
-  </si>
-  <si>
-    <t>finance_is_processing_fee_verified</t>
-  </si>
-  <si>
-    <t>finance_is_inspection_fee_verified</t>
-  </si>
-  <si>
-    <t>inspection_status</t>
-  </si>
-  <si>
-    <t>are_equipment_and_monitoring_fees_verified</t>
-  </si>
-  <si>
-    <t>area_officer_approval</t>
-  </si>
-  <si>
-    <t>hod_marine_approval</t>
-  </si>
-  <si>
-    <t>employer_id</t>
-  </si>
-  <si>
-    <t>29/29/08</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Service ID</t>
+  </si>
+  <si>
+    <t>Service Type ID</t>
+  </si>
+  <si>
+    <t>Applicant ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Application_Form_Payment_Status</t>
+  </si>
+  <si>
+    <t>Date_Of_Inspection</t>
+  </si>
+  <si>
+    <t>Current_Step</t>
+  </si>
+  <si>
+    <t>MSE_Are_Documents_Verified</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Finance_Is_Application_Fee_Verified</t>
+  </si>
+  <si>
+    <t>Finance_Is_Processing_Fee_Verified</t>
+  </si>
+  <si>
+    <t>Finance_Is_Inspection_Fee_Verified</t>
+  </si>
+  <si>
+    <t>Inspection Status</t>
+  </si>
+  <si>
+    <t>Are Equipment And Monitoring Fees Verified</t>
+  </si>
+  <si>
+    <t>Area_Officer_Approval</t>
+  </si>
+  <si>
+    <t>Marine_Hod_Approval</t>
   </si>
 </sst>
 </file>
@@ -76,7 +73,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -118,7 +115,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,15 +399,16 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30.109375" bestFit="1" customWidth="1"/>
@@ -423,13 +421,13 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -438,31 +436,31 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
         <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -472,17 +470,17 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
+      <c r="C2">
+        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
+        <v>44958</v>
+      </c>
+      <c r="F2">
         <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
       </c>
       <c r="G2">
         <v>0</v>

</xml_diff>

<commit_message>
done with the modification of the excelsheet and upload data
</commit_message>
<xml_diff>
--- a/public/excelfile/serviceapplication.xlsx
+++ b/public/excelfile/serviceapplication.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5844"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9252"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Service ID</t>
   </si>
@@ -65,7 +65,13 @@
     <t>Area_Officer_Approval</t>
   </si>
   <si>
-    <t>Marine_Hod_Approval</t>
+    <t>mechanical</t>
+  </si>
+  <si>
+    <t>manual</t>
+  </si>
+  <si>
+    <t>Hod_Approval</t>
   </si>
 </sst>
 </file>
@@ -396,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -460,7 +466,7 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -470,14 +476,14 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>13</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" s="2">
-        <v>44958</v>
+        <v>44928</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -504,6 +510,47 @@
         <v>1</v>
       </c>
       <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>44928</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed the service application and employer
</commit_message>
<xml_diff>
--- a/public/excelfile/serviceapplication.xlsx
+++ b/public/excelfile/serviceapplication.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Service ID</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Service Type ID</t>
   </si>
   <si>
-    <t>Applicant ID</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Application_Form_Payment_Status</t>
   </si>
   <si>
@@ -72,6 +69,12 @@
   </si>
   <si>
     <t>Hod_Approval</t>
+  </si>
+  <si>
+    <t>Applicant code</t>
+  </si>
+  <si>
+    <t>NIRC6633540063e77</t>
   </si>
 </sst>
 </file>
@@ -404,8 +407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,7 +430,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -436,48 +439,48 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="N1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>16</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -514,14 +517,14 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
+      <c r="A3" t="s">
+        <v>16</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>1</v>

</xml_diff>